<commit_message>
Ajout du résidentiel 2D
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_residentiel_2D_bis.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_residentiel_2D_bis.xlsx
@@ -1088,13 +1088,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3296205</v>
+        <v>320487</v>
       </c>
       <c r="D2" t="n">
-        <v>239.8445075447252</v>
+        <v>239.4219237582472</v>
       </c>
       <c r="E2" t="n">
-        <v>156.3396158376272</v>
+        <v>66.95905227218795</v>
       </c>
     </row>
     <row r="3">
@@ -1256,13 +1256,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7003032</v>
+        <v>3775624</v>
       </c>
       <c r="D10" t="n">
-        <v>276.9415384914412</v>
+        <v>274.568821693265</v>
       </c>
       <c r="E10" t="n">
-        <v>138.7559571931911</v>
+        <v>112.8278356336831</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
notebook update w bug
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_residentiel_2D_bis.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_residentiel_2D_bis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07A9F12-2C17-9F43-8799-758091472D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{A07A9F12-2C17-9F43-8799-758091472D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D28DC733-C84C-4BDF-BB12-490DA543104A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
@@ -473,11 +473,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,7 +490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -493,7 +498,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -501,7 +506,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -509,7 +514,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -528,9 +533,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -562,7 +567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -594,7 +599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -626,7 +631,7 @@
         <v>0.72104118463674227</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -658,7 +663,7 @@
         <v>0.56914728682170546</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -690,7 +695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -722,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -754,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -786,7 +791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -829,9 +834,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -848,7 +853,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -865,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -882,7 +887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -899,7 +904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -916,7 +921,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -933,7 +938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -950,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -967,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -993,16 +998,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1019,7 +1024,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1036,7 +1041,7 @@
         <v>66.959052272187947</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1053,7 +1058,7 @@
         <v>68.656688977716797</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1070,7 +1075,7 @@
         <v>66.283435853153662</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1087,7 +1092,7 @@
         <v>62.634561091350477</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1104,7 +1109,7 @@
         <v>52.973740041026069</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1121,7 +1126,7 @@
         <v>44.438915275434461</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1138,7 +1143,7 @@
         <v>10.255134294331031</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1155,7 +1160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1172,7 +1177,7 @@
         <v>112.82783563368309</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1189,7 +1194,7 @@
         <v>116.852067445918</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1206,7 +1211,7 @@
         <v>109.2501764322046</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1223,7 +1228,7 @@
         <v>86.516098080883552</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1240,7 +1245,7 @@
         <v>105.71703104202599</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1257,7 +1262,7 @@
         <v>92.499838314799049</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1274,7 +1279,7 @@
         <v>21.3461165341844</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1302,9 +1307,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1312,7 +1317,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1320,7 +1325,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>

</xml_diff>